<commit_message>
add html5 & git
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +39,22 @@
   </si>
   <si>
     <t>http://www.99css.com/cssgaga/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTML5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://e.jikexueyuan.com/html5.html?hmsr=baidu_sem_html5_dy_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.liaoxuefeng.com/wiki/0013739516305929606dd18361248578c67b8067c8c017b000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -630,13 +646,13 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="B2:D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="32.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
@@ -665,13 +681,21 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="2:4">

</xml_diff>